<commit_message>
Update data. Minor bugfixes and refactorings
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,22 +1,310 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowWidth="28800" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="215">
+  <si>
+    <t>arise</t>
+  </si>
+  <si>
+    <t>arose</t>
+  </si>
+  <si>
+    <t>arisen</t>
+  </si>
+  <si>
+    <t>Phát sinh</t>
+  </si>
+  <si>
+    <t>awake</t>
+  </si>
+  <si>
+    <t>awoke, awaked</t>
+  </si>
+  <si>
+    <t>awoken, awaked</t>
+  </si>
+  <si>
+    <t>Đánh thức, thức</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>was, were</t>
+  </si>
+  <si>
+    <t>been</t>
+  </si>
+  <si>
+    <t>Thì, là, ở</t>
+  </si>
+  <si>
+    <t>bear</t>
+  </si>
+  <si>
+    <t>bore</t>
+  </si>
+  <si>
+    <t>borne</t>
+  </si>
+  <si>
+    <t>Mang, chịu đựng</t>
+  </si>
+  <si>
+    <t>beat</t>
+  </si>
+  <si>
+    <t>beaten, beat</t>
+  </si>
+  <si>
+    <t>Đánh, đánh bại</t>
+  </si>
+  <si>
+    <t>become</t>
+  </si>
+  <si>
+    <t>became</t>
+  </si>
+  <si>
+    <t>Trở nên</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>began</t>
+  </si>
+  <si>
+    <t>begun</t>
+  </si>
+  <si>
+    <t>Bắt đầu</t>
+  </si>
+  <si>
+    <t>bend</t>
+  </si>
+  <si>
+    <t>bent</t>
+  </si>
+  <si>
+    <t>Bẻ cong, cuối xuống</t>
+  </si>
+  <si>
+    <t>bind</t>
+  </si>
+  <si>
+    <t>bound</t>
+  </si>
+  <si>
+    <t>Buộc, trói</t>
+  </si>
+  <si>
+    <t>bite</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>bitten</t>
+  </si>
+  <si>
+    <t>Cắn, ngoạm</t>
+  </si>
+  <si>
+    <t>bleed</t>
+  </si>
+  <si>
+    <t>bled</t>
+  </si>
+  <si>
+    <t>Chảy máu</t>
+  </si>
+  <si>
+    <t>bless</t>
+  </si>
+  <si>
+    <t>blessed</t>
+  </si>
+  <si>
+    <t>blessed, blest</t>
+  </si>
+  <si>
+    <t>Ban phước lành</t>
+  </si>
+  <si>
+    <t>blow</t>
+  </si>
+  <si>
+    <t>blew</t>
+  </si>
+  <si>
+    <t>blown</t>
+  </si>
+  <si>
+    <t>Thổi</t>
+  </si>
+  <si>
+    <t>break</t>
+  </si>
+  <si>
+    <t>broke</t>
+  </si>
+  <si>
+    <t>broken</t>
+  </si>
+  <si>
+    <t>Vỡ, đạp vỡ</t>
+  </si>
+  <si>
+    <t>breed</t>
+  </si>
+  <si>
+    <t>bred</t>
+  </si>
+  <si>
+    <t>Nuôi, dạy dỗ</t>
+  </si>
+  <si>
+    <t>bring</t>
+  </si>
+  <si>
+    <t>brought</t>
+  </si>
+  <si>
+    <t>Mang đến</t>
+  </si>
+  <si>
+    <t>broadcast</t>
+  </si>
+  <si>
+    <t>Phát thanh</t>
+  </si>
+  <si>
+    <t>build</t>
+  </si>
+  <si>
+    <t>built</t>
+  </si>
+  <si>
+    <t>Xây dựng</t>
+  </si>
+  <si>
+    <t>burn</t>
+  </si>
+  <si>
+    <t>burnt, burned</t>
+  </si>
+  <si>
+    <t>Đốt, cháy</t>
+  </si>
+  <si>
+    <t>burst</t>
+  </si>
+  <si>
+    <t>Nổ tung</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>bought</t>
+  </si>
+  <si>
+    <t>Mua</t>
+  </si>
+  <si>
+    <t>cast</t>
+  </si>
+  <si>
+    <t>Ném, tung</t>
+  </si>
+  <si>
+    <t>catch</t>
+  </si>
+  <si>
+    <t>caught</t>
+  </si>
+  <si>
+    <t>Bắt, chụp</t>
+  </si>
+  <si>
+    <t>choose</t>
+  </si>
+  <si>
+    <t>chose</t>
+  </si>
+  <si>
+    <t>chosen</t>
+  </si>
+  <si>
+    <t>Chọn, lựa</t>
+  </si>
+  <si>
+    <t>cling</t>
+  </si>
+  <si>
+    <t>clung</t>
+  </si>
+  <si>
+    <t>Bám chặt</t>
+  </si>
+  <si>
+    <t>come</t>
+  </si>
+  <si>
+    <t>came</t>
+  </si>
+  <si>
+    <t>Đến</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>Trị giá</t>
+  </si>
+  <si>
+    <t>creep</t>
+  </si>
+  <si>
+    <t>crept</t>
+  </si>
+  <si>
+    <t>Bò</t>
+  </si>
+  <si>
+    <t>crow</t>
+  </si>
+  <si>
+    <t>crew, crowed</t>
+  </si>
+  <si>
+    <t>crowed</t>
+  </si>
+  <si>
+    <t>Gáy</t>
+  </si>
+  <si>
+    <t>cut</t>
+  </si>
+  <si>
+    <t>Cắt</t>
+  </si>
   <si>
     <t>deal</t>
   </si>
@@ -378,23 +666,187 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,8 +859,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -418,77 +1056,318 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -779,21 +1658,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" ht="31.5" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -801,515 +1683,973 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
+    <row r="2" ht="47.25" spans="1:6">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" ht="31.5" spans="1:6">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" ht="47.25" spans="1:6">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" ht="31.5" spans="1:6">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" ht="15.75" spans="1:6">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" ht="15.75" spans="1:6">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" ht="47.25" spans="1:6">
+      <c r="A8" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" ht="31.5" spans="1:6">
+      <c r="A9" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" ht="31.5" spans="1:6">
+      <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" ht="31.5" spans="1:6">
+      <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" ht="47.25" spans="1:6">
+      <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>40</v>
+      <c r="C12" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" ht="15.75" spans="1:6">
+      <c r="A13" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" ht="31.5" spans="1:6">
+      <c r="A14" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" ht="31.5" spans="1:6">
+      <c r="A15" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" ht="31.5" spans="1:6">
+      <c r="A16" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" ht="31.5" spans="1:6">
+      <c r="A17" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" ht="31.5" spans="1:6">
+      <c r="A18" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" ht="31.5" spans="1:6">
+      <c r="A19" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" ht="15.75" spans="1:6">
+      <c r="A20" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" ht="15.75" spans="1:6">
+      <c r="A21" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="C21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" ht="31.5" spans="1:6">
+      <c r="A22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" ht="31.5" spans="1:6">
+      <c r="A23" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" ht="31.5" spans="1:6">
+      <c r="A24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" ht="31.5" spans="1:6">
+      <c r="A25" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="C25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" ht="15.75" spans="1:6">
+      <c r="A26" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="C26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" ht="15.75" spans="1:6">
+      <c r="A27" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" ht="15.75" spans="1:6">
+      <c r="A28" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" ht="31.5" spans="1:6">
+      <c r="A29" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" ht="15.75" spans="1:6">
+      <c r="A30" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="B30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" ht="31.5" spans="1:4">
+      <c r="A31" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="B31" s="6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="C31" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="2" t="s">
+    </row>
+    <row r="32" ht="15.75" spans="1:4">
+      <c r="A32" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="B32" s="6" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="C32" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="2" t="s">
+    </row>
+    <row r="33" ht="15.75" spans="1:4">
+      <c r="A33" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="B33" s="6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="C33" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="D33" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="2" t="s">
+    </row>
+    <row r="34" ht="15.75" spans="1:4">
+      <c r="A34" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="B34" s="6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="C34" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="D34" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="2" t="s">
+    </row>
+    <row r="35" ht="31.5" spans="1:4">
+      <c r="A35" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="B35" s="6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="C35" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="2" t="s">
+    </row>
+    <row r="36" ht="15.75" spans="1:4">
+      <c r="A36" s="6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="B36" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C36" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="D36" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="37" ht="15.75" spans="1:4">
+      <c r="A37" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="B37" s="6" t="s">
         <v>118</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" ht="31.5" spans="1:4">
+      <c r="A38" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" spans="1:4">
+      <c r="A39" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" spans="1:4">
+      <c r="A40" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" ht="31.5" spans="1:4">
+      <c r="A41" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" ht="31.5" spans="1:4">
+      <c r="A42" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" ht="31.5" spans="1:4">
+      <c r="A43" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" spans="1:4">
+      <c r="A44" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" ht="31.5" spans="1:4">
+      <c r="A45" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" ht="31.5" spans="1:4">
+      <c r="A46" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" spans="1:4">
+      <c r="A47" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" ht="31.5" spans="1:4">
+      <c r="A48" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" ht="47.25" spans="1:4">
+      <c r="A49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" ht="31.5" spans="1:4">
+      <c r="A50" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" ht="31.5" spans="1:4">
+      <c r="A51" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" ht="31.5" spans="1:4">
+      <c r="A52" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" spans="1:4">
+      <c r="A53" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="54" ht="15.75" spans="1:4">
+      <c r="A54" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" ht="31.5" spans="1:4">
+      <c r="A55" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" ht="31.5" spans="1:4">
+      <c r="A56" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" spans="1:4">
+      <c r="A57" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" ht="31.5" spans="1:4">
+      <c r="A58" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" ht="15.75" spans="1:4">
+      <c r="A59" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="60" ht="31.5" spans="1:4">
+      <c r="A60" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="61" ht="31.5" spans="1:4">
+      <c r="A61" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" spans="1:4">
+      <c r="A62" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" spans="1:4">
+      <c r="A63" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" ht="31.5" spans="1:4">
+      <c r="A64" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" ht="15.75" spans="1:4">
+      <c r="A65" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>